<commit_message>
Completed Question #2. Done for now.
</commit_message>
<xml_diff>
--- a/transfusion_data.xlsx
+++ b/transfusion_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/550518d20e19b26c/Desktop/MBiotech/Classes/BTC1877/Team Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/550518d20e19b26c/Documents/BTC1877_team_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_8483295C020366DB1F6185675263248952F1800B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17F4A054-8C34-4A8A-A9EE-992AAAED3A8F}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_8483295C020366DB1F6185675263248952F1800B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5439705-4DD3-497C-A9EA-0D2B1E6733EB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -916,6 +916,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1241,10 +1245,10 @@
   <dimension ref="A1:DM201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BC2" sqref="BC2"/>
+      <selection pane="bottomRight" activeCell="AL10" sqref="AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>

</xml_diff>